<commit_message>
- Cresus.Database: amélioration du logging. - AIDER: le logging peut être activé au moyen d'une directive EnableDbConsoleLogger dans le fichier .crconfig.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@24043 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="103">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -307,6 +307,30 @@
   </si>
   <si>
     <t>Divers, réponses aux mails, etc.</t>
+  </si>
+  <si>
+    <t>Déploiement 1.4.1446.0 + RCH</t>
+  </si>
+  <si>
+    <t>Chasse au bug, analyse registre</t>
+  </si>
+  <si>
+    <t>Gestion des déf. De groupes "fonctions"</t>
+  </si>
+  <si>
+    <t>Analyse Registres</t>
+  </si>
+  <si>
+    <t>Export BN + maintenance</t>
+  </si>
+  <si>
+    <t>Analyse, médlisation, modifications</t>
+  </si>
+  <si>
+    <t>Collaborateurs AIDER</t>
+  </si>
+  <si>
+    <t>Utilisateurs AIDER</t>
   </si>
 </sst>
 </file>
@@ -720,7 +744,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,8 +811,16 @@
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>41957</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
       <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -798,8 +830,16 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>41963</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
       <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -809,8 +849,15 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="1">
+        <v>41967</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1011,8 +1058,15 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="1">
+        <v>41954</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F25" s="8"/>
       <c r="G25" s="2">
         <f t="shared" si="2"/>
@@ -1023,8 +1077,15 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="1">
+        <v>41956</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="2">
         <f t="shared" si="2"/>
@@ -1035,8 +1096,15 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="1">
+        <v>41962</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="F27" s="8"/>
       <c r="G27" s="2">
         <f t="shared" si="2"/>
@@ -1047,8 +1115,15 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="1">
+        <v>41968</v>
+      </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="2">
         <f t="shared" si="2"/>
@@ -1059,8 +1134,15 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="1">
+        <v>41969</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="2">
         <f t="shared" si="2"/>
@@ -1071,8 +1153,15 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
+      <c r="B30" s="1">
+        <v>41970</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="2">
         <f t="shared" si="2"/>
@@ -1140,11 +1229,11 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.22222222222222221</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0</v>
+        <v>9.722222222222221E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1164,11 +1253,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.22222222222222221</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>5.333333333333333</v>
+        <v>32</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1180,7 +1269,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>800</v>
+        <v>4800</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
- DataLayer: amélioré la performance du LoaderQueryGenerator (facteur 70) quand les entités rapatriées ont beaucoup de collections; Firebird n'arrive pas à utiliser les index pour un SELECT ... WHERE (x IN (SELECT ...)) alors que cela fonctionne avec SELECT ... WHERE (x IN (...)). - DataLayer: ajouté un cache des clés primaires dans Request.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@24050 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="106">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>Utilisateurs AIDER</t>
+  </si>
+  <si>
+    <t>Renommages de collab./chgmt gestion/région</t>
+  </si>
+  <si>
+    <t>Analyse lenteurs AIDER</t>
+  </si>
+  <si>
+    <t>Amélioration performance SUB-SELECT</t>
   </si>
 </sst>
 </file>
@@ -744,7 +753,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,30 +876,57 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="1">
+        <v>41974</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5972222222222224E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="1">
+        <v>41975</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="1">
+        <v>41977</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1172,8 +1208,15 @@
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
+      <c r="B31" s="1">
+        <v>41975</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.25</v>
+      </c>
       <c r="G31" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1229,7 +1272,7 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>1.3333333333333335</v>
+        <v>1.9444444444444444</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1238,7 +1281,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="13">
         <f>SUM(G4:G37)</f>
-        <v>0</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="13">
@@ -1253,11 +1296,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>1.3333333333333335</v>
+        <v>1.7951388888888888</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>32</v>
+        <v>43.083333333333336</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1269,7 +1312,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>4800</v>
+        <v>6462.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
- DataLayer: corrigé problème avec requête utilisée plus d'une fois. - AIDER: mis à jour la doc.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@24078 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="108">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>Amélioration performance SUB-SELECT</t>
+  </si>
+  <si>
+    <t>Registres</t>
+  </si>
+  <si>
+    <t>Correctif pour mailings</t>
   </si>
 </sst>
 </file>
@@ -753,7 +759,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,8 +942,15 @@
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="1">
+        <v>41984</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1226,8 +1239,15 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="1">
+        <v>41982</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="F32" s="8"/>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
@@ -1272,7 +1292,7 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>1.9444444444444444</v>
+        <v>2.3125</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1296,11 +1316,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>1.7951388888888888</v>
+        <v>2.1631944444444446</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>43.083333333333336</v>
+        <v>51.916666666666664</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1312,7 +1332,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>6462.5</v>
+        <v>7787.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
- Aider: version 1.4.1451.0. - Aider: complété les traductions manquantes pour AiderEvent.Kind et Participants.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@24103 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="109">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Correctif pour mailings</t>
+  </si>
+  <si>
+    <t>Registres, étiquettes pour ministres</t>
   </si>
 </sst>
 </file>
@@ -759,7 +762,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,8 +963,15 @@
       <c r="A12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="1">
+        <v>41988</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G12" s="2">
         <f t="shared" ref="G12:G35" si="1">D12*F12</f>
         <v>0</v>
@@ -1258,8 +1268,15 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="1">
+        <v>41983</v>
+      </c>
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="F33" s="8"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
@@ -1270,8 +1287,15 @@
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="1">
+        <v>41984</v>
+      </c>
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.25694444444444448</v>
+      </c>
       <c r="F34" s="8"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
@@ -1282,8 +1306,15 @@
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
+      <c r="B35" s="1">
+        <v>41988</v>
+      </c>
+      <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1292,7 +1323,7 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>2.3125</v>
+        <v>3.0208333333333335</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1316,11 +1347,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>2.1631944444444446</v>
+        <v>2.8715277777777781</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>51.916666666666664</v>
+        <v>68.916666666666671</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1332,7 +1363,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>7787.5</v>
+        <v>10337.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
- Lignes de commandes.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@24148 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/2014-05-xx.xlsx
@@ -7,22 +7,23 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2014.45-48" sheetId="9" r:id="rId1"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId2"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId3"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId4"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId5"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId6"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
+    <sheet name="2015.01" sheetId="10" r:id="rId1"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId2"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId3"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId4"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId5"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId6"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId7"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="110">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -349,6 +350,9 @@
   </si>
   <si>
     <t>Registres, étiquettes pour ministres</t>
+  </si>
+  <si>
+    <t>Registres, ajouter une personne à un acte</t>
   </si>
 </sst>
 </file>
@@ -762,7 +766,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,17 +815,10 @@
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>41954</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="D4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G11" si="0">D4*F4</f>
+        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
         <v>0</v>
       </c>
     </row>
@@ -829,16 +826,9 @@
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>41957</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -848,16 +838,9 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>41963</v>
-      </c>
-      <c r="C6" t="s">
-        <v>99</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -867,15 +850,8 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>41967</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" s="2"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -885,57 +861,30 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>41974</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.5</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>6.5972222222222224E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>41975</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.5</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>41977</v>
-      </c>
-      <c r="C10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="2">
-        <v>6.25E-2</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -945,15 +894,8 @@
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1">
-        <v>41984</v>
-      </c>
-      <c r="C11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -963,17 +905,10 @@
       <c r="A12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1">
-        <v>41988</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G35" si="1">D12*F12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -984,7 +919,7 @@
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -995,7 +930,7 @@
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1006,7 +941,7 @@
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1017,7 +952,7 @@
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G16:G29" si="1">D16*F16</f>
         <v>0</v>
       </c>
     </row>
@@ -1080,17 +1015,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>41947</v>
+        <v>41982</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D23" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G31" si="2">D23*F23</f>
+        <f t="shared" ref="G23:G26" si="2">D23*F23</f>
         <v>0</v>
       </c>
     </row>
@@ -1099,13 +1034,13 @@
         <v>13</v>
       </c>
       <c r="B24" s="1">
-        <v>41949</v>
+        <v>41983</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D24" s="2">
-        <v>4.1666666666666664E-2</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="2">
@@ -1118,13 +1053,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="1">
-        <v>41954</v>
+        <v>41984</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D25" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.25694444444444448</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="2">
@@ -1137,13 +1072,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="1">
-        <v>41956</v>
+        <v>41988</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="D26" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="2">
@@ -1156,17 +1091,17 @@
         <v>13</v>
       </c>
       <c r="B27" s="1">
-        <v>41962</v>
+        <v>41996</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D27" s="2">
-        <v>0.10416666666666667</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1174,18 +1109,11 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1">
-        <v>41968</v>
-      </c>
-      <c r="C28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.20833333333333334</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
       <c r="F28" s="8"/>
       <c r="G28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1193,18 +1121,11 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1">
-        <v>41969</v>
-      </c>
-      <c r="C29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
       <c r="F29" s="8"/>
       <c r="G29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1212,18 +1133,11 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1">
-        <v>41970</v>
-      </c>
-      <c r="C30" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.16666666666666666</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
       <c r="F30" s="8"/>
       <c r="G30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G30:G35" si="3">D30*F30</f>
         <v>0</v>
       </c>
     </row>
@@ -1231,17 +1145,10 @@
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1">
-        <v>41975</v>
-      </c>
-      <c r="C31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.25</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1249,18 +1156,11 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="1">
-        <v>41982</v>
-      </c>
-      <c r="C32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
       <c r="F32" s="8"/>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1268,18 +1168,11 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1">
-        <v>41983</v>
-      </c>
-      <c r="C33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
       <c r="F33" s="8"/>
       <c r="G33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1287,18 +1180,11 @@
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="1">
-        <v>41984</v>
-      </c>
-      <c r="C34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.25694444444444448</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
       <c r="F34" s="8"/>
       <c r="G34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1306,33 +1192,26 @@
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="1">
-        <v>41988</v>
-      </c>
-      <c r="C35" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.1388888888888889</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>3.0208333333333335</v>
+        <v>1.0625</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>9.722222222222221E-2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
         <f>SUM(G4:G37)</f>
-        <v>0.14930555555555555</v>
+        <v>0</v>
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="13">
@@ -1347,11 +1226,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>2.8715277777777781</v>
+        <v>1.0625</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>68.916666666666671</v>
+        <v>25.5</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1363,7 +1242,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>10337.5</v>
+        <v>3825</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1430,7 +1309,667 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41954</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G11" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41957</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41963</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41967</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41974</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.2916666666666671E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41975</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41977</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41984</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41988</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" ref="G12:G35" si="1">D12*F12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41947</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G31" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41949</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41954</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41956</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41962</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41968</v>
+      </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41969</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>41970</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>41975</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.020833333333333</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>9.722222222222221E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.864583333333333</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>44.75</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>6712.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2048,7 +2587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2687,7 +3226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3349,7 +3888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3887,7 +4426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4453,7 +4992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5019,18 +5558,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>

</xml_diff>